<commit_message>
feat: Added notebook for Webinar Python
</commit_message>
<xml_diff>
--- a/Fasttrack/Episode_2/Paint_Sales_Regression.xlsx
+++ b/Fasttrack/Episode_2/Paint_Sales_Regression.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vreed\Desktop\Ryan\AIEngineer\WGU\MSDA\D208_Predictive_Modeling\Fasttrack\Episode_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EADB9F-8A53-4633-9844-5810339B2439}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CAA2F5-C601-49B3-A515-CC5ACFBAE071}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B481C1CA-B254-4BC4-8B8F-27EA678710B6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Paint Sales</t>
   </si>
@@ -43,14 +43,106 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
+  </si>
+  <si>
+    <t>RESIDUAL OUTPUT</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>Residuals</t>
+  </si>
+  <si>
+    <t>Predicted Volume</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -66,7 +158,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -74,12 +166,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -95,6 +215,604 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Price  Residual Plot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$40:$G$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>17.931718936085701</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-8.5113140134974401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-15.843588725684867</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.39737991266378</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.9380706629614224</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5.7264787614133184</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.6089718142119409</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8669-4668-8782-D0EA009CD06C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1000215456"/>
+        <c:axId val="1000215040"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1000215456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Price</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1000215040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1000215040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Residuals</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1000215456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Price Line Fit  Plot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Volume</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>425</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>310</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A42B-4F92-8BDC-E42B9AB58A9C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Predicted Volume</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$40:$F$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>482.0682810639143</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>458.51131401349744</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>440.84358872568487</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>411.39737991266378</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>376.06192933703858</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>340.72647876141332</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>305.39102818578806</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A42B-4F92-8BDC-E42B9AB58A9C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="823488928"/>
+        <c:axId val="823489760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="823488928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Price</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="823489760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="823489760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Volume</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="823488928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="18" name="Chart 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2DE1E14-E99B-4C9A-B67C-CD88EF66E2F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>819149</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="19" name="Chart 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEDB8C88-1EA6-42F2-B1CF-3338BF37999E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -394,20 +1112,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38ADF894-4806-4283-96DF-21AFFDB00A17}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -415,7 +1140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>500</v>
       </c>
@@ -423,7 +1148,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>450</v>
       </c>
@@ -431,15 +1156,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>425</v>
       </c>
       <c r="B5">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>410</v>
       </c>
@@ -447,7 +1172,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>385</v>
       </c>
@@ -455,7 +1180,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>335</v>
       </c>
@@ -463,7 +1188,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>310</v>
       </c>
@@ -471,7 +1196,317 @@
         <v>48</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.98471617430179259</v>
+      </c>
+    </row>
+    <row r="20" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.96966594393155847</v>
+      </c>
+    </row>
+    <row r="21" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.96359913271787012</v>
+      </c>
+    </row>
+    <row r="22" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="1">
+        <v>12.497081834838953</v>
+      </c>
+    </row>
+    <row r="23" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E26" s="3"/>
+      <c r="F26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <v>24961.971870923837</v>
+      </c>
+      <c r="H27" s="1">
+        <v>24961.971870923837</v>
+      </c>
+      <c r="I27" s="1">
+        <v>159.83123749487046</v>
+      </c>
+      <c r="J27" s="1">
+        <v>5.5013442941896754E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1">
+        <v>5</v>
+      </c>
+      <c r="G28" s="1">
+        <v>780.88527193330879</v>
+      </c>
+      <c r="H28" s="1">
+        <v>156.17705438666175</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="2">
+        <v>6</v>
+      </c>
+      <c r="G29" s="2">
+        <v>25742.857142857145</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="1">
+        <v>588.07463279079002</v>
+      </c>
+      <c r="G32" s="1">
+        <v>15.446862312538686</v>
+      </c>
+      <c r="H32" s="1">
+        <v>38.0708146995932</v>
+      </c>
+      <c r="I32" s="1">
+        <v>2.3557973466034758E-7</v>
+      </c>
+      <c r="J32" s="1">
+        <v>548.36720911260295</v>
+      </c>
+      <c r="K32" s="1">
+        <v>627.78205646897709</v>
+      </c>
+      <c r="L32" s="1">
+        <v>548.36720911260295</v>
+      </c>
+      <c r="M32" s="1">
+        <v>627.78205646897709</v>
+      </c>
+    </row>
+    <row r="33" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F33" s="2">
+        <v>-5.8892417626042075</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.4658311777100832</v>
+      </c>
+      <c r="H33" s="2">
+        <v>-12.64243795693182</v>
+      </c>
+      <c r="I33" s="2">
+        <v>5.5013442941896754E-5</v>
+      </c>
+      <c r="J33" s="2">
+        <v>-7.0866989264988192</v>
+      </c>
+      <c r="K33" s="2">
+        <v>-4.6917845987095959</v>
+      </c>
+      <c r="L33" s="2">
+        <v>-7.0866989264988192</v>
+      </c>
+      <c r="M33" s="2">
+        <v>-4.6917845987095959</v>
+      </c>
+    </row>
+    <row r="37" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E40" s="1">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1">
+        <v>482.0682810639143</v>
+      </c>
+      <c r="G40" s="1">
+        <v>17.931718936085701</v>
+      </c>
+    </row>
+    <row r="41" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E41" s="1">
+        <v>2</v>
+      </c>
+      <c r="F41" s="1">
+        <v>458.51131401349744</v>
+      </c>
+      <c r="G41" s="1">
+        <v>-8.5113140134974401</v>
+      </c>
+    </row>
+    <row r="42" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E42" s="1">
+        <v>3</v>
+      </c>
+      <c r="F42" s="1">
+        <v>440.84358872568487</v>
+      </c>
+      <c r="G42" s="1">
+        <v>-15.843588725684867</v>
+      </c>
+    </row>
+    <row r="43" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E43" s="1">
+        <v>4</v>
+      </c>
+      <c r="F43" s="1">
+        <v>411.39737991266378</v>
+      </c>
+      <c r="G43" s="1">
+        <v>-1.39737991266378</v>
+      </c>
+    </row>
+    <row r="44" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E44" s="1">
+        <v>5</v>
+      </c>
+      <c r="F44" s="1">
+        <v>376.06192933703858</v>
+      </c>
+      <c r="G44" s="1">
+        <v>8.9380706629614224</v>
+      </c>
+    </row>
+    <row r="45" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E45" s="1">
+        <v>6</v>
+      </c>
+      <c r="F45" s="1">
+        <v>340.72647876141332</v>
+      </c>
+      <c r="G45" s="1">
+        <v>-5.7264787614133184</v>
+      </c>
+    </row>
+    <row r="46" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E46" s="2">
+        <v>7</v>
+      </c>
+      <c r="F46" s="2">
+        <v>305.39102818578806</v>
+      </c>
+      <c r="G46" s="2">
+        <v>4.6089718142119409</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J40:J46">
+    <sortCondition ref="J40"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>